<commit_message>
Analisis y muestra no comentarios
</commit_message>
<xml_diff>
--- a/Result_df/df_postss.xlsx
+++ b/Result_df/df_postss.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K57"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,20 +490,20 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.397980001161601e+18</v>
+        <v>1.399735901618676e+18</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>AT_USER Haciendo gestiones...</t>
+          <t>AT_USER haha jonathan you are banging mostopapi</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>-0.2872256228337421</v>
+        <v>-0.598635256446478</v>
       </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
@@ -523,20 +523,21 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1.397976717306876e+18</v>
+        <v>1.39972896705835e+18</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>AT_USER Espabila con Lis</t>
+          <t>Q mostopapi ha hecho un hábitos con la asquerosa de la ex de mario
+Q hace dandole fama a esa podrida</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1.752272378191661</v>
       </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
@@ -556,20 +557,20 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1.397172544885645e+18</v>
+        <v>1.39972230554735e+18</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Lo de pasar rapido los audios de wasa es lo mejor</t>
+          <t>AT_USER Estas preparado para el habitos con mostopapi?</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0.8790333783564991</v>
+        <v>-0.737051996900189</v>
       </c>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
@@ -589,20 +590,20 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>1.396257002800693e+18</v>
+        <v>1.399722024516399e+18</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Tocara ir a ver saww</t>
+          <t>AT_USER AT_USER AT_USER AT_USER AT_USER AT_USER AT_USER AT_USER AT_USER https://t.co/L4c62PsDkA</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>-1.137231677157825</v>
+        <v>0.6492423642197017</v>
       </c>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
@@ -622,20 +623,20 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>1.396230674542121e+18</v>
+        <v>1.399721444003693e+18</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>De lo cos</t>
+          <t>AT_USER AT_USER AT_USER AT_USER AT_USER AT_USER AT_USER AT_USER AT_USER https://t.co/47TANT6qrt</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>-1.653342728774344</v>
+        <v>0.6492423642197017</v>
       </c>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
@@ -655,20 +656,20 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1.394666359141847e+18</v>
+        <v>1.399720783744803e+18</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>AT_USER JAJAJAJAJAJAJAJAJAJAJAJAJAAJAJAJAJAJAJAJAJAJAJAJAJAJA</t>
+          <t>Cuántas veces habéis cancelado ya al Grefg ese? Pa qué lo hacéis si se os olvida a los 4 días? En qué quedó la canc… https://t.co/oMyfI855W0</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>-2.218651514604828</v>
       </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
@@ -688,20 +689,20 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>1.393950120664879e+18</v>
+        <v>1.399719960201552e+18</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Regalando dinero a la urban🤑</t>
+          <t>Contraataque de twich ASMR a los hot tubs, sobar los microfonos... Mostopapi adelantado por la derecha</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>-1.02473406935197</v>
+        <v>1.416724213713826</v>
       </c>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
@@ -721,20 +722,20 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>1.393305669688775e+18</v>
+        <v>1.399706881510236e+18</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>AT_USER 🌚👌🏻</t>
+          <t>AT_USER mostopapi youtuber de toda la vida?</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>-0.7809568132404325</v>
+        <v>-0.1494140261201318</v>
       </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
@@ -754,20 +755,21 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>1.393300041851408e+18</v>
+        <v>1.399706298997002e+18</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>He convertido a mi hermana en una posadora fitness 💁🏻‍♂️</t>
+          <t>Dato curioso:
+No es para justificar nada ni mucho menos pero... Os habéis fijado que últimamente los grandes youtub… https://t.co/VytJuVCLo6</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>-0.7509834102645365</v>
+        <v>0.005291538171256827</v>
       </c>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
@@ -787,20 +789,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>1.392957179645334e+18</v>
+        <v>1.399705586535735e+18</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>AT_USER AT_USER Soy yo capullo 🥲</t>
+          <t>AT_USER Mujer: pene vagina
+Mostopapi: *glup*
+Niños de 13 años:</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>-1.777090163428478</v>
       </c>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
@@ -820,11 +824,11 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>1.392953588486484e+18</v>
+        <v>1.399687555214459e+18</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>AT_USER AT_USER</t>
+          <t>AT_USER AT_USER Ejem ejem mostopapi</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -853,20 +857,20 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>1.392244774170681e+18</v>
+        <v>1.399681109894574e+18</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Chiklin</t>
+          <t>mostopapi cuando salga sexo 2 https://t.co/0SlFkfcfos</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>0.6936045046476975</v>
       </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
@@ -886,20 +890,22 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>1.391166456168059e+18</v>
+        <v>1.399665997532078e+18</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Homemade fmUab</t>
+          <t>MUCHAS GRACIAS AT_USER 😍
+Es el MEJOR ✨ día de mi VIDA. Pronto haremos un hábitos tu y yo😎🥵🤭
+Es INDESCRPTIBLE 😱 e… https://t.co/RHGsFbVyJI</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>7.662528096930197</v>
       </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
@@ -919,20 +925,20 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>1.390557884975653e+18</v>
+        <v>1.399659729878716e+18</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Madrugaciones</t>
+          <t>Cuando parece que no puede ser más imbécil, Mostopapi te demuestra que si puede y que estábamos equivocados. https://t.co/WTbFVYe57Z</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>1.468094515427772</v>
       </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
@@ -952,11 +958,12 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>1.390060154360586e+18</v>
+        <v>1.399656284509643e+18</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>AT_USER Pillado 🌚🤌🏻</t>
+          <t>Un año de universidad: Sobre 1000€
+Un año seguido por Mostopapi: 1200€ y ganarte el status de pajero supremo.</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -965,7 +972,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>-0.737051996900189</v>
+        <v>-1.807293319241956</v>
       </c>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
@@ -985,20 +992,21 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>1.389260722656457e+18</v>
+        <v>1.399655874013143e+18</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>AT_USER https://t.co/RuyG0gL9eX</t>
+          <t>Comprarse la entrada del primavera: mentalidad de pobre
+Esperar a que sortee una mostopapi: mentalidad de tiburón</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>-3.333039390911592</v>
       </c>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
@@ -1018,20 +1026,20 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>1.389260171722072e+18</v>
+        <v>1.399648158800658e+18</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>AT_USER Te dije que te callaras 👍🏻</t>
+          <t>AT_USER AT_USER mostopapi, para empezar</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>-2.616621098808731</v>
+        <v>0</v>
       </c>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
@@ -1051,20 +1059,20 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>1.388975692545724e+18</v>
+        <v>1.399563450263736e+18</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>AT_USER 5€?</t>
+          <t>no le veo la gracia a los videos d mostopapi jsjsa hernan se duerme en vivo</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>-0.0439048163402436</v>
+        <v>5.84254243795721</v>
       </c>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
@@ -1084,11 +1092,11 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>1.388964723392135e+18</v>
+        <v>1.399513599467573e+18</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>AT_USER Callate un poco</t>
+          <t>AT_USER Aunq mostopapi tienw sida</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1117,20 +1125,20 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>1.388096505559622e+18</v>
+        <v>1.399507040658145e+18</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Mis ojos van por caminos separados en las fotos xd</t>
+          <t>100 pavos para que mostopapi te tenga muted https://t.co/fRKWnCu55g</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>-1.120066456607234</v>
+        <v>-0.449369924448408</v>
       </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
@@ -1150,20 +1158,20 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>1.388096414211838e+18</v>
+        <v>1.399503069398852e+18</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>No se puede salir peor</t>
+          <t>oye AT_USER hazte un video con Hashim Thaçi, primer presidente de Kosovo tras la independecia e imputado por cri… https://t.co/FfgCX2fDoJ</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>-1.486442344172787</v>
+        <v>1.879720087274797</v>
       </c>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
@@ -1183,20 +1191,20 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>1.387909008305136e+18</v>
+        <v>1.399499650781045e+18</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>AT_USER 🤟🏻😔🤟🏻</t>
+          <t>AT_USER AT_USER Q va me referia a mostopapi</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>-2.211155990700567</v>
+        <v>0.1198297320977574</v>
       </c>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr"/>
@@ -1216,20 +1224,20 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>1.387902102945534e+18</v>
+        <v>1.39948515584528e+18</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Quiero comer como un cerdo pero toca definir :(</t>
+          <t>AT_USER AT_USER Willyrex y mostopapi 😍</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>-11.4775637562015</v>
+        <v>0</v>
       </c>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr"/>
@@ -1249,11 +1257,11 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>1.387495857059254e+18</v>
+        <v>1.399484475424268e+18</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>AT_USER el tt noseke ahjahja</t>
+          <t>100 euros o mes porque te siga Mostopapi , é o proxeneta mais barato da historia https://t.co/Z63QpsgYu8</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1262,7 +1270,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>0.4421408025170406</v>
       </c>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
@@ -1282,20 +1290,22 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>1.387490031603003e+18</v>
+        <v>1.399482560527442e+18</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>AT_USER Hoy, no fallamos papifabri😛</t>
+          <t>-¿Papá me das 100€ para material escolar?
+-Tu también has visto lo de Mostopapi eh
+-Sí https://t.co/NG3YHddyhK</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>0.2643965433142731</v>
+        <v>-2.250973714902479</v>
       </c>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
@@ -1315,20 +1325,20 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>1.387488811488268e+18</v>
+        <v>1.399471026703057e+18</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>El viernes orleamos✌🏻</t>
+          <t>AT_USER AT_USER AT_USER</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>1.546320892343985</v>
+        <v>0</v>
       </c>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr"/>
@@ -1348,20 +1358,21 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>1.386135208244785e+18</v>
+        <v>1.399467459720225e+18</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>AT_USER Tremenda F</t>
+          <t>https://t.co/0C9URCuLfC
+mostopapi era un principiante a su lado, a mi lo de este canal un dia me lo tienen que expl… https://t.co/0AVpI8zl9c</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>0.3615602917679208</v>
+        <v>2.615318595547004</v>
       </c>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
@@ -1381,20 +1392,20 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>1.386126225974993e+18</v>
+        <v>1.399466123138114e+18</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>A la mierda el horario 🤗</t>
+          <t>Como molaría un hábitos con AT_USER AT_USER 🤔</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>-2.110092760520375</v>
+        <v>0</v>
       </c>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
@@ -1414,20 +1425,20 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>1.385373695812768e+18</v>
+        <v>1.399463091193233e+18</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>AT_USER 🤟🏻😔🤟🏻</t>
+          <t>AT_USER Puto mostopapi siempre liándola</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>-2.211155990700567</v>
+        <v>-0.006164488357396644</v>
       </c>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr"/>
@@ -1447,20 +1458,20 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>1.38537334787838e+18</v>
+        <v>1.399458315944579e+18</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>AT_USER https://t.co/JqF119gaLZ</t>
+          <t>¿Qué leyes INCUMPLE el SORTEO de MOSTOPAPI e ITRADEIT? Feat. AT_USER y Deso... https://t.co/nyM5EUvp0f a través de AT_USER</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>0</v>
+        <v>-1.894861009258642</v>
       </c>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr"/>
@@ -1480,20 +1491,21 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>1.384819462327652e+18</v>
+        <v>1.399454229467697e+18</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>AT_USER Me tocara hacerte carrito en todo, nada nuevo 🤡</t>
+          <t>mostopapi
+mostopapi cuando salga sexo 2 https://t.co/c4xOrvODsK</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>-0.2801815253279433</v>
+        <v>0.6936045046476975</v>
       </c>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr"/>
@@ -1513,11 +1525,11 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>1.38425262739583e+18</v>
+        <v>1.399444678852948e+18</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>AT_USER Gracias precioso 😚😚</t>
+          <t>AT_USER AT_USER A ver cómo cojones me mantengo sin comida para las próximas 3 semanas</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1526,7 +1538,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>1.763541933749813</v>
+        <v>0.8234325000537276</v>
       </c>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr"/>
@@ -1546,11 +1558,11 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>1.384248847325561e+18</v>
+        <v>1.399444208545677e+18</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>A ver todas las pelis d marvel prq n tengo na mejor q hacer 🤓</t>
+          <t>AT_USER AT_USER AT_USER AT_USER Un año de derecho o un año de mostopapi nose tú pero yo lo tengo claro jajaja</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1559,7 +1571,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>2.593552242692311</v>
+        <v>1.801313674360861</v>
       </c>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr"/>
@@ -1579,20 +1591,20 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>1.383487764675531e+18</v>
+        <v>1.399442673258439e+18</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Y ya me ha pasao</t>
+          <t>AT_USER Que pensabas que te iba a regalar mostopapi, una cruz de Cristo?</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>-2.434299542014776</v>
       </c>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr"/>
@@ -1612,20 +1624,20 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>1.380966258858996e+18</v>
+        <v>1.399439868455969e+18</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Bien lo de dejar a uno de 1.60 cubrir un palo</t>
+          <t>AT_USER Grande Mostopapi</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>-1.360775308493374</v>
+        <v>0.3615602917679208</v>
       </c>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
@@ -1645,20 +1657,20 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>1.379040941919633e+18</v>
+        <v>1.399439276799111e+18</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>AT_USER Dutxat porc AT_USER</t>
+          <t>AT_USER El putísimo Mostopapi me ha regalado un puto pajeador que poco le falta para tener función de decirte te q… https://t.co/bGjLpewePT</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>-0.7791398696366406</v>
       </c>
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr"/>
@@ -1678,20 +1690,20 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>1.378427621294346e+18</v>
+        <v>1.399439183614288e+18</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Cortame mas el pelo si eso ehhhh</t>
+          <t>El putísimo Mostopapi me ha regalado un puto pajeador que poco le falta para tener función de decirte te quiero y a… https://t.co/pt1qdnm4LX</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>0.7809984615055402</v>
+        <v>-3.46949049363945</v>
       </c>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr"/>
@@ -1711,20 +1723,20 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>1.378383274079351e+18</v>
+        <v>1.399435544195748e+18</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>AT_USER AT_USER</t>
+          <t>AT_USER AT_USER Jajajajajaja y en el mostopapi xk bro? No estoy muy al tanto recientemente de lo q sube n… https://t.co/Jf7w6zpMXW</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>0</v>
+        <v>1.520830024062756</v>
       </c>
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr"/>
@@ -1744,11 +1756,11 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>1.377692233009402e+18</v>
+        <v>1.399433451682636e+18</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>AT_USER Cabron llevas piripa todo el dia</t>
+          <t>Es del Monopoly x Mostopapi  llevo tiempo buscandolo 🤩 https://t.co/XhOdXtIQD7</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1757,7 +1769,7 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>-0.963278370034387</v>
+        <v>-1.069825972347302</v>
       </c>
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr"/>
@@ -1777,20 +1789,20 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>1.375173169208758e+18</v>
+        <v>1.399428948094751e+18</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>El muesli de casa ametller es lo puto mejor</t>
+          <t>Mostopapi me da como pereza</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>-0.3339892614893547</v>
+        <v>-0.5547304401062343</v>
       </c>
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr"/>
@@ -1810,20 +1822,20 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>1.374832748867768e+18</v>
+        <v>1.399428075708891e+18</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Q asco me da mi compañero de trabajo de la uni d vd no hace el puto huevo</t>
+          <t>AT_USER AT_USER Voy a ello yo también, los 100 leuros mejor invertidos</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>0.08717451547556454</v>
+        <v>3.17452021905323</v>
       </c>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr"/>
@@ -1843,20 +1855,20 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>1.374467791433036e+18</v>
+        <v>1.399427455404941e+18</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Verdades como puños</t>
+          <t>JOJOJOJO que 100 euros más bien gastados, gracias ídolo AT_USER https://t.co/GdjTcQrRgw</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>0.1102458634870147</v>
+        <v>2.993033790702265</v>
       </c>
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr"/>
@@ -1876,20 +1888,20 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>1.374465162049069e+18</v>
+        <v>1.399427089711964e+18</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Nacho wapo</t>
+          <t>AT_USER ahhora yo tambien quiero que le haga la entrevista mostopapi</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
+        <v>-1.361892492587509</v>
       </c>
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr"/>
@@ -1909,20 +1921,20 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>1.374130548394881e+18</v>
+        <v>1.399426942722523e+18</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Me apetece sushi y vino blanco🥲</t>
+          <t>AT_USER AT_USER Es más ha pagado 105€ gran seguidor</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>-1.679696662137248</v>
+        <v>3.947111509070813</v>
       </c>
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr"/>
@@ -1942,11 +1954,11 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>1.374103562901459e+18</v>
+        <v>1.39942556388277e+18</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Sigo esperando</t>
+          <t>Me he dejado todos mis ahorros en el follow de Mostopapi https://t.co/mDkJCNMSt9</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1955,7 +1967,7 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>0.3176554754276771</v>
+        <v>-0.449369924448408</v>
       </c>
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr"/>
@@ -1975,20 +1987,20 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>1.374040255989432e+18</v>
+        <v>1.399425453820191e+18</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>AT_USER Borratxo</t>
+          <t>mostopapi hazle una entrevista a powerbazinga por favor es lo unico que te voy a pedir</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>0</v>
+        <v>-1.600534468740906</v>
       </c>
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr"/>
@@ -2008,20 +2020,20 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>1.373999600365879e+18</v>
+        <v>1.399422495187509e+18</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Coffeeeeee</t>
+          <t>AT_USER AT_USER no nos jodas la vida eh q nos quedamos tiesos</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>0</v>
+        <v>0.9668978396473789</v>
       </c>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr"/>
@@ -2041,11 +2053,11 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>1.372329788933804e+18</v>
+        <v>1.399418403950141e+18</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>AT_USER Llevo casi dos mesus esperan</t>
+          <t>AT_USER Sien euros mostopapi culo teta xoxo</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -2054,7 +2066,7 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>-0.7634059302630936</v>
+        <v>-1.741152361454831</v>
       </c>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr"/>
@@ -2074,20 +2086,20 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>1.372329468317078e+18</v>
+        <v>1.399416884542517e+18</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Quiero mis nike yaaaaaaaa que salga mi numero porfavor</t>
+          <t>AT_USER AT_USER Umtiti y mostopapi</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>-2.416599964915376</v>
+        <v>0</v>
       </c>
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr"/>
@@ -2107,20 +2119,20 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>1.370935215137362e+18</v>
+        <v>1.399416576521159e+18</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Alutas?</t>
+          <t>AT_USER AT_USER Mostopapi también es vasco aparte de Guinea Ecuatorial, pero bueno, como tú quieras.</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>0</v>
+        <v>0.8963676888415413</v>
       </c>
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr"/>
@@ -2135,204 +2147,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="B52" t="n">
-        <v>1.370863064967447e+18</v>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>AT_USER Descansa precioso 💕</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>Negative</t>
-        </is>
-      </c>
-      <c r="E52" t="n">
-        <v>-2.32893902635695</v>
-      </c>
-      <c r="F52" t="inlineStr"/>
-      <c r="G52" t="inlineStr"/>
-      <c r="H52" t="inlineStr"/>
-      <c r="I52" t="n">
-        <v>0</v>
-      </c>
-      <c r="J52" t="n">
-        <v>0</v>
-      </c>
-      <c r="K52" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="1" t="n">
-        <v>51</v>
-      </c>
-      <c r="B53" t="n">
-        <v>1.37077825887103e+18</v>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>Me siento: 🤡</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>Negative</t>
-        </is>
-      </c>
-      <c r="E53" t="n">
-        <v>-2.569633460648499</v>
-      </c>
-      <c r="F53" t="inlineStr"/>
-      <c r="G53" t="inlineStr"/>
-      <c r="H53" t="inlineStr"/>
-      <c r="I53" t="n">
-        <v>0</v>
-      </c>
-      <c r="J53" t="n">
-        <v>0</v>
-      </c>
-      <c r="K53" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="1" t="n">
-        <v>52</v>
-      </c>
-      <c r="B54" t="n">
-        <v>1.370110477213258e+18</v>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>AT_USER https://t.co/nacJnaVx3e</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
-      </c>
-      <c r="E54" t="n">
-        <v>0</v>
-      </c>
-      <c r="F54" t="inlineStr"/>
-      <c r="G54" t="inlineStr"/>
-      <c r="H54" t="inlineStr"/>
-      <c r="I54" t="n">
-        <v>0</v>
-      </c>
-      <c r="J54" t="n">
-        <v>0</v>
-      </c>
-      <c r="K54" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="1" t="n">
-        <v>53</v>
-      </c>
-      <c r="B55" t="n">
-        <v>1.369784040291721e+18</v>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>Echo d menos el cine d mi pueblo :(</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>Negative</t>
-        </is>
-      </c>
-      <c r="E55" t="n">
-        <v>-1.180156708789894</v>
-      </c>
-      <c r="F55" t="inlineStr"/>
-      <c r="G55" t="inlineStr"/>
-      <c r="H55" t="inlineStr"/>
-      <c r="I55" t="n">
-        <v>0</v>
-      </c>
-      <c r="J55" t="n">
-        <v>0</v>
-      </c>
-      <c r="K55" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="1" t="n">
-        <v>54</v>
-      </c>
-      <c r="B56" t="n">
-        <v>1.369385027650388e+18</v>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>Who knows</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
-      </c>
-      <c r="E56" t="n">
-        <v>0</v>
-      </c>
-      <c r="F56" t="inlineStr"/>
-      <c r="G56" t="inlineStr"/>
-      <c r="H56" t="inlineStr"/>
-      <c r="I56" t="n">
-        <v>0</v>
-      </c>
-      <c r="J56" t="n">
-        <v>0</v>
-      </c>
-      <c r="K56" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="B57" t="n">
-        <v>1.368977262536757e+18</v>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>Hoy d negro</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
-      </c>
-      <c r="E57" t="n">
-        <v>5.391522668242771</v>
-      </c>
-      <c r="F57" t="inlineStr"/>
-      <c r="G57" t="inlineStr"/>
-      <c r="H57" t="inlineStr"/>
-      <c r="I57" t="n">
-        <v>0</v>
-      </c>
-      <c r="J57" t="n">
-        <v>0</v>
-      </c>
-      <c r="K57" t="n">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
botones y graficos bien
</commit_message>
<xml_diff>
--- a/Result_df/df_postss.xlsx
+++ b/Result_df/df_postss.xlsx
@@ -490,20 +490,20 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.399735901618676e+18</v>
+        <v>1.399853305464041e+18</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>AT_USER haha jonathan you are banging mostopapi</t>
+          <t>AT_USER Cause the dick is better</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>-0.598635256446478</v>
+        <v>0.4718061552549353</v>
       </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
@@ -523,21 +523,20 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1.39972896705835e+18</v>
+        <v>1.399853303681405e+18</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Q mostopapi ha hecho un hábitos con la asquerosa de la ex de mario
-Q hace dandole fama a esa podrida</t>
+          <t>AT_USER Fat ass to balance the fat dick?</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1.752272378191661</v>
+        <v>0.4718061552549353</v>
       </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
@@ -557,11 +556,11 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1.39972230554735e+18</v>
+        <v>1.399853300623741e+18</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>AT_USER Estas preparado para el habitos con mostopapi?</t>
+          <t>I remember I said some shit along these lines several years back and that dirty looking asshole from Philly who cla… https://t.co/Cps87fGruy</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -570,7 +569,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>-0.737051996900189</v>
+        <v>-2.319879387926461</v>
       </c>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
@@ -590,20 +589,20 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>1.399722024516399e+18</v>
+        <v>1.399853300313436e+18</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>AT_USER AT_USER AT_USER AT_USER AT_USER AT_USER AT_USER AT_USER AT_USER https://t.co/L4c62PsDkA</t>
+          <t>And don’t forget cuz they broke!! Dick ride/Kiss Ass to ride ya wave!! Some mf wouldn’t drink if not for ppl buying… https://t.co/B0zvDIlZPD</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.6492423642197017</v>
+        <v>-0.9705074919657545</v>
       </c>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
@@ -623,20 +622,20 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>1.399721444003693e+18</v>
+        <v>1.399853286975578e+18</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>AT_USER AT_USER AT_USER AT_USER AT_USER AT_USER AT_USER AT_USER AT_USER https://t.co/47TANT6qrt</t>
+          <t>big dick small heart</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0.6492423642197017</v>
+        <v>-0.8248616295806762</v>
       </c>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
@@ -656,11 +655,11 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1.399720783744803e+18</v>
+        <v>1.399853283309765e+18</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Cuántas veces habéis cancelado ya al Grefg ese? Pa qué lo hacéis si se os olvida a los 4 días? En qué quedó la canc… https://t.co/oMyfI855W0</t>
+          <t>AT_USER AT_USER I am as soon as I get home. I look like Shrek-it-Ralph, and guarantee I have at least 3 i… https://t.co/haHYF6c0D3</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -669,7 +668,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>-2.218651514604828</v>
+        <v>-4.783598356628086</v>
       </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
@@ -689,20 +688,20 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>1.399719960201552e+18</v>
+        <v>1.399853282789581e+18</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Contraataque de twich ASMR a los hot tubs, sobar los microfonos... Mostopapi adelantado por la derecha</t>
+          <t>I need you to be on my dick but I can also get tired of you fast 🥴</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>1.416724213713826</v>
+        <v>-1.027357903202228</v>
       </c>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
@@ -722,20 +721,21 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>1.399706881510236e+18</v>
+        <v>1.399853279656489e+18</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>AT_USER mostopapi youtuber de toda la vida?</t>
+          <t>Hmmm
+I wanna suck a dick</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>-0.1494140261201318</v>
+        <v>-1.12300058430516</v>
       </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
@@ -755,21 +755,20 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>1.399706298997002e+18</v>
+        <v>1.399853279434232e+18</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Dato curioso:
-No es para justificar nada ni mucho menos pero... Os habéis fijado que últimamente los grandes youtub… https://t.co/VytJuVCLo6</t>
+          <t>this boy added me to his paid private snap for free and i never see him give head or some fingering po, it's always… https://t.co/de1Gd7sdRR</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>0.005291538171256827</v>
+        <v>1.003965243327911</v>
       </c>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
@@ -789,13 +788,12 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>1.399705586535735e+18</v>
+        <v>1.399853278691828e+18</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>AT_USER Mujer: pene vagina
-Mostopapi: *glup*
-Niños de 13 años:</t>
+          <t>Send £10 then Drop a heavy book on your dick &amp;amp; send me proof 😂
+Findom cbt</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -804,7 +802,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>-1.777090163428478</v>
+        <v>-0.6942118141339159</v>
       </c>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
@@ -824,20 +822,20 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>1.399687555214459e+18</v>
+        <v>1.399853274161893e+18</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>AT_USER AT_USER Ejem ejem mostopapi</t>
+          <t>AT_USER AT_USER AT_USER AT_USER AT_USER literally suck dick??? like your stalking our pa… https://t.co/1KPa0Yc2HM</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>-2.129066586585657</v>
       </c>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
@@ -857,20 +855,21 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>1.399681109894574e+18</v>
+        <v>1.399853270470783e+18</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>mostopapi cuando salga sexo 2 https://t.co/0SlFkfcfos</t>
+          <t>All these white boys in downtown Los Angeles California on Crystal meth an suck each others dick..
+Stay away from downtown white boys...</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>0.6936045046476975</v>
+        <v>-1.338313625548617</v>
       </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
@@ -890,22 +889,20 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>1.399665997532078e+18</v>
+        <v>1.399853259356058e+18</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>MUCHAS GRACIAS AT_USER 😍
-Es el MEJOR ✨ día de mi VIDA. Pronto haremos un hábitos tu y yo😎🥵🤭
-Es INDESCRPTIBLE 😱 e… https://t.co/RHGsFbVyJI</t>
+          <t>Small dick energy https://t.co/MK6YmPXrxb</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>7.662528096930197</v>
+        <v>-1.474103993800378</v>
       </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
@@ -925,11 +922,12 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>1.399659729878716e+18</v>
+        <v>1.399853258559181e+18</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Cuando parece que no puede ser más imbécil, Mostopapi te demuestra que si puede y que estábamos equivocados. https://t.co/WTbFVYe57Z</t>
+          <t>So horny, any girls want to see my big white cock? Like or DM me 🍆
+#cock #dick #dickrate #cumtribute #cocktribute… https://t.co/0RCeIRI80z</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -938,7 +936,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>1.468094515427772</v>
+        <v>1.59588723727359</v>
       </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
@@ -958,21 +956,20 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>1.399656284509643e+18</v>
+        <v>1.399853257535767e+18</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Un año de universidad: Sobre 1000€
-Un año seguido por Mostopapi: 1200€ y ganarte el status de pajero supremo.</t>
+          <t>it’s the end of my dick dn era ✊🏽😔</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>-1.807293319241956</v>
+        <v>0.427066458178303</v>
       </c>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
@@ -992,21 +989,20 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>1.399655874013143e+18</v>
+        <v>1.399853255501533e+18</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Comprarse la entrada del primavera: mentalidad de pobre
-Esperar a que sortee una mostopapi: mentalidad de tiburón</t>
+          <t>AT_USER // They are but my Kol is a dick. 😂 https://t.co/z19CJQjDJ4</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>-3.333039390911592</v>
+        <v>-0.08292428485129894</v>
       </c>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
@@ -1026,20 +1022,20 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>1.399648158800658e+18</v>
+        <v>1.399853252762604e+18</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>AT_USER AT_USER mostopapi, para empezar</t>
+          <t>AT_USER You must have a really small dick.</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>-1.335687253346667</v>
       </c>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
@@ -1059,20 +1055,20 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>1.399563450263736e+18</v>
+        <v>1.399853249868362e+18</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>no le veo la gracia a los videos d mostopapi jsjsa hernan se duerme en vivo</t>
+          <t>AT_USER I’ll suck that lady dick nice</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>5.84254243795721</v>
+        <v>-0.4298534037452152</v>
       </c>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
@@ -1092,20 +1088,20 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>1.399513599467573e+18</v>
+        <v>1.399853248530596e+18</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>AT_USER Aunq mostopapi tienw sida</t>
+          <t>AT_USER AT_USER Damn just ask him don’t have to suck his dick</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>0.8145496858293204</v>
       </c>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
@@ -1125,20 +1121,20 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>1.399507040658145e+18</v>
+        <v>1.399853245003178e+18</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>100 pavos para que mostopapi te tenga muted https://t.co/fRKWnCu55g</t>
+          <t>hoes a dick ride to make a  friend pathetic 😂😂😂😂😂😂😂😂😂😂😂😂😂😂😂😂😂😂😂😂😂😂😂😂😂😂😂😂😂😂😂😂</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>-0.449369924448408</v>
+        <v>-2.512769476516695</v>
       </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
@@ -1158,11 +1154,11 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>1.399503069398852e+18</v>
+        <v>1.399853243623043e+18</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>oye AT_USER hazte un video con Hashim Thaçi, primer presidente de Kosovo tras la independecia e imputado por cri… https://t.co/FfgCX2fDoJ</t>
+          <t>AT_USER AT_USER Yeah, I know you'd never do something out of spite, and it's certainly harmless. I just imme… https://t.co/1kDoTZCFVs</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1171,7 +1167,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>1.879720087274797</v>
+        <v>0.6319480692872864</v>
       </c>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
@@ -1191,20 +1187,20 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>1.399499650781045e+18</v>
+        <v>1.399853238514602e+18</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>AT_USER AT_USER Q va me referia a mostopapi</t>
+          <t>AT_USER dick é melhor q o jason e o bruce???</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>0.1198297320977574</v>
+        <v>-0.8248616295806762</v>
       </c>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr"/>
@@ -1224,20 +1220,21 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>1.39948515584528e+18</v>
+        <v>1.399853235029037e+18</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>AT_USER AT_USER Willyrex y mostopapi 😍</t>
+          <t>First deep tweet pog,
+ive found that I've made a lot more friends online recently! they're all awesome!! but I thi… https://t.co/kc0pYKzxBp</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>1.14056504017783</v>
       </c>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr"/>
@@ -1257,11 +1254,11 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>1.399484475424268e+18</v>
+        <v>1.399853233200407e+18</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>100 euros o mes porque te siga Mostopapi , é o proxeneta mais barato da historia https://t.co/Z63QpsgYu8</t>
+          <t>Get some dick and go don’t go to claiming no nigga kids and all this. Especially not mine cause my job is handled.</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1270,7 +1267,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>0.4421408025170406</v>
+        <v>0.009486880309583223</v>
       </c>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
@@ -1290,13 +1287,11 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>1.399482560527442e+18</v>
+        <v>1.399853215441637e+18</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>-¿Papá me das 100€ para material escolar?
--Tu también has visto lo de Mostopapi eh
--Sí https://t.co/NG3YHddyhK</t>
+          <t>I got that dick that make you go “I mean I guess that works”</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1305,7 +1300,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>-2.250973714902479</v>
+        <v>-5.164380691756528</v>
       </c>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
@@ -1325,20 +1320,20 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>1.399471026703057e+18</v>
+        <v>1.399853212849541e+18</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>AT_USER AT_USER AT_USER</t>
+          <t>I hate when I get good dick and then can’t have it again :..(</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>-3.540866427436733</v>
       </c>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr"/>
@@ -1358,21 +1353,20 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>1.399467459720225e+18</v>
+        <v>1.399853210446316e+18</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>https://t.co/0C9URCuLfC
-mostopapi era un principiante a su lado, a mi lo de este canal un dia me lo tienen que expl… https://t.co/0AVpI8zl9c</t>
+          <t>Future wife sai ame pass out on some dick</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>2.615318595547004</v>
+        <v>-0.9126712622611632</v>
       </c>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
@@ -1392,20 +1386,20 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>1.399466123138114e+18</v>
+        <v>1.399853205748687e+18</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Como molaría un hábitos con AT_USER AT_USER 🤔</t>
+          <t>AT_USER Can a dick fit in your mouth?</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>-1.923473918248786</v>
       </c>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
@@ -1425,20 +1419,20 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>1.399463091193233e+18</v>
+        <v>1.399853202397295e+18</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>AT_USER Puto mostopapi siempre liándola</t>
+          <t>I’ve been accused of discriminatory hiring practices in my role as Floor Manager at the dick sucking factory.</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>-0.006164488357396644</v>
+        <v>0.5607465449248874</v>
       </c>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr"/>
@@ -1458,11 +1452,12 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>1.399458315944579e+18</v>
+        <v>1.399853200417509e+18</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>¿Qué leyes INCUMPLE el SORTEO de MOSTOPAPI e ITRADEIT? Feat. AT_USER y Deso... https://t.co/nyM5EUvp0f a través de AT_USER</t>
+          <t>Every time I see someone post a photo with a sleeping cat on them say “how am I gonna move now 🤪” i get mad
+Try it… https://t.co/ecA7UuoDRn</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1471,7 +1466,7 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>-1.894861009258642</v>
+        <v>-1.484547303177751</v>
       </c>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr"/>
@@ -1491,21 +1486,20 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>1.399454229467697e+18</v>
+        <v>1.399853190514946e+18</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>mostopapi
-mostopapi cuando salga sexo 2 https://t.co/c4xOrvODsK</t>
+          <t>AT_USER Many levels dick head.</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>0.6936045046476975</v>
+        <v>-0.737051996900189</v>
       </c>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr"/>
@@ -1525,20 +1519,20 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>1.399444678852948e+18</v>
+        <v>1.39985318413541e+18</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>AT_USER AT_USER A ver cómo cojones me mantengo sin comida para las próximas 3 semanas</t>
+          <t>AT_USER idk. hey AT_USER How much more propaganda until Dick automatically becomes the fifth?</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>0.8234325000537276</v>
+        <v>-0.2446121368479259</v>
       </c>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr"/>
@@ -1558,20 +1552,20 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>1.399444208545677e+18</v>
+        <v>1.399853172361925e+18</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>AT_USER AT_USER AT_USER AT_USER Un año de derecho o un año de mostopapi nose tú pero yo lo tengo claro jajaja</t>
+          <t>AT_USER AT_USER I smell jealousy, attention and need dick to chill tf out okay hanna leave my whore tana alone</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>1.801313674360861</v>
+        <v>-0.1811907998044897</v>
       </c>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr"/>
@@ -1591,11 +1585,11 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>1.399442673258439e+18</v>
+        <v>1.39985316852403e+18</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>AT_USER Que pensabas que te iba a regalar mostopapi, una cruz de Cristo?</t>
+          <t>AT_USER AT_USER i fucking saw that LMAOOO “come on my dick”</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1604,7 +1598,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>-2.434299542014776</v>
+        <v>-2.196093820346754</v>
       </c>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr"/>
@@ -1624,20 +1618,20 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>1.399439868455969e+18</v>
+        <v>1.399853166993318e+18</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>AT_USER Grande Mostopapi</t>
+          <t>He wants to suck Trumps dick sooooooooooooo badly https://t.co/CnosXBF3yX</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>0.3615602917679208</v>
+        <v>-1.23032673768884</v>
       </c>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
@@ -1657,11 +1651,12 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>1.399439276799111e+18</v>
+        <v>1.399853166162854e+18</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>AT_USER El putísimo Mostopapi me ha regalado un puto pajeador que poco le falta para tener función de decirte te q… https://t.co/bGjLpewePT</t>
+          <t>I know she suck dick 
+I know she ain’t shit</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1670,7 +1665,7 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>-0.7791398696366406</v>
+        <v>-3.500581080709481</v>
       </c>
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr"/>
@@ -1690,11 +1685,11 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>1.399439183614288e+18</v>
+        <v>1.399853164359193e+18</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>El putísimo Mostopapi me ha regalado un puto pajeador que poco le falta para tener función de decirte te quiero y a… https://t.co/pt1qdnm4LX</t>
+          <t>AT_USER AT_USER A useless dick</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1703,7 +1698,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>-3.46949049363945</v>
+        <v>-0.737051996900189</v>
       </c>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr"/>
@@ -1723,20 +1718,20 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>1.399435544195748e+18</v>
+        <v>1.399853158331929e+18</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>AT_USER AT_USER Jajajajajaja y en el mostopapi xk bro? No estoy muy al tanto recientemente de lo q sube n… https://t.co/Jf7w6zpMXW</t>
+          <t>“Dick is like a drug”😂</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>1.520830024062756</v>
+        <v>-2.211155990700567</v>
       </c>
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr"/>
@@ -1756,11 +1751,11 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>1.399433451682636e+18</v>
+        <v>1.399853156905927e+18</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Es del Monopoly x Mostopapi  llevo tiempo buscandolo 🤩 https://t.co/XhOdXtIQD7</t>
+          <t>The cute guy i’ve been flirting with hit me with the “hey i cant flirt anymore i’m in a relationship” text 😔😔😔 one less dick for me</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1769,7 +1764,7 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>-1.069825972347302</v>
+        <v>-3.957866313703584</v>
       </c>
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr"/>
@@ -1789,11 +1784,11 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>1.399428948094751e+18</v>
+        <v>1.399853148152467e+18</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Mostopapi me da como pereza</t>
+          <t>AT_USER I was like "Yay she's back, awww look at the bunny...............................Shit that's a nice di… https://t.co/JGRN65DSsr</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1802,7 +1797,7 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>-0.5547304401062343</v>
+        <v>-2.66202153036146</v>
       </c>
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr"/>
@@ -1822,20 +1817,20 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>1.399428075708891e+18</v>
+        <v>1.399853144541176e+18</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>AT_USER AT_USER Voy a ello yo también, los 100 leuros mejor invertidos</t>
+          <t>AT_USER Baby you've got my dick about to explode</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>3.17452021905323</v>
+        <v>-1.630906497967817</v>
       </c>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr"/>
@@ -1855,11 +1850,11 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>1.399427455404941e+18</v>
+        <v>1.399853135074513e+18</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>JOJOJOJO que 100 euros más bien gastados, gracias ídolo AT_USER https://t.co/GdjTcQrRgw</t>
+          <t>AT_USER It's just assholes who want to dick ride other people's personal experiences for clout. Some people have zero shame.</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1868,7 +1863,7 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>2.993033790702265</v>
+        <v>0.5475013181748671</v>
       </c>
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr"/>
@@ -1888,20 +1883,20 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>1.399427089711964e+18</v>
+        <v>1.39985313312009e+18</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>AT_USER ahhora yo tambien quiero que le haga la entrevista mostopapi</t>
+          <t>I wish my squirting dildo didn't make a fizzing sort of sound when it ejaculates, but it does and there doesn't see… https://t.co/lNMBhw9dOX</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>-1.361892492587509</v>
+        <v>-0.3568100651654639</v>
       </c>
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr"/>
@@ -1921,20 +1916,20 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>1.399426942722523e+18</v>
+        <v>1.399853130616037e+18</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>AT_USER AT_USER Es más ha pagado 105€ gran seguidor</t>
+          <t>AT_USER Idk if I wanna suck your tits or dick first</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>3.947111509070813</v>
+        <v>-3.364129977981624</v>
       </c>
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr"/>
@@ -1954,20 +1949,20 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>1.39942556388277e+18</v>
+        <v>1.399853122437059e+18</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Me he dejado todos mis ahorros en el follow de Mostopapi https://t.co/mDkJCNMSt9</t>
+          <t>AT_USER AT_USER He has my vote for “Dick of the decade”.</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>-0.449369924448408</v>
+        <v>0.9642460153071983</v>
       </c>
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr"/>
@@ -1987,11 +1982,11 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>1.399425453820191e+18</v>
+        <v>1.399853111561294e+18</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>mostopapi hazle una entrevista a powerbazinga por favor es lo unico que te voy a pedir</t>
+          <t>AT_USER AT_USER AT_USER Lmao he was a dick head to me too, I liked to describe him as thinking h… https://t.co/QTZL3Xun5p</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -2000,7 +1995,7 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>-1.600534468740906</v>
+        <v>-3.695716866773648</v>
       </c>
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr"/>
@@ -2020,20 +2015,20 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>1.399422495187509e+18</v>
+        <v>1.399853109871059e+18</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>AT_USER AT_USER no nos jodas la vida eh q nos quedamos tiesos</t>
+          <t>AT_USER &amp;amp; I be son more onnuh dick soooooo</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>0.9668978396473789</v>
+        <v>-1.816147764865106</v>
       </c>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr"/>
@@ -2053,11 +2048,11 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>1.399418403950141e+18</v>
+        <v>1.399853109396922e+18</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>AT_USER Sien euros mostopapi culo teta xoxo</t>
+          <t>Oh shit happy pride month 😳 I like dick but I’m scared of it</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -2066,7 +2061,7 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>-1.741152361454831</v>
+        <v>-4.740755909609097</v>
       </c>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr"/>
@@ -2086,20 +2081,20 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>1.399416884542517e+18</v>
+        <v>1.399853107660485e+18</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>AT_USER AT_USER Umtiti y mostopapi</t>
+          <t>AT_USER Patriot dick wad: no thanks I have a headache.</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>0</v>
+        <v>-1.728338132184619</v>
       </c>
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr"/>
@@ -2119,20 +2114,20 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>1.399416576521159e+18</v>
+        <v>1.399853106016526e+18</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>AT_USER AT_USER Mostopapi también es vasco aparte de Guinea Ecuatorial, pero bueno, como tú quieras.</t>
+          <t>AT_USER What zero dick does to a person</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>0.8963676888415413</v>
+        <v>-0.3754917051322682</v>
       </c>
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr"/>

</xml_diff>